<commit_message>
Diagramas de robustez y registro de tiempo al hacerlos
En este commit se subieron los diagramas de robustez de los casos de uso 14,15,16,21, así como el registro del tiempo que se llevo en su elaboración.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
+++ b/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Dropbox\Proyecto Desarrollo de Software\plantillas\Iteración 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E08D53-47C3-4132-8746-DD79E5ED99FD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
   <si>
     <t>Columna</t>
   </si>
@@ -347,6 +346,9 @@
   </si>
   <si>
     <t>Modelo de dominio (40%)</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -619,12 +621,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,6 +667,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1022,10 @@
   <dimension ref="B1:BA100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="S57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,84 +1100,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="51"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="35"/>
+      <c r="O4" s="51"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="35"/>
+      <c r="R4" s="51"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="34" t="s">
+      <c r="T4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="35"/>
+      <c r="U4" s="51"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="34" t="s">
+      <c r="W4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="35"/>
+      <c r="X4" s="51"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="34" t="s">
+      <c r="Z4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="35"/>
+      <c r="AA4" s="51"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AC4" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="35"/>
+      <c r="AD4" s="51"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="34" t="s">
+      <c r="AF4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="35"/>
+      <c r="AG4" s="51"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="34" t="s">
+      <c r="AI4" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="35"/>
+      <c r="AJ4" s="51"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="35"/>
+      <c r="AM4" s="51"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="34" t="s">
+      <c r="AO4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="35"/>
+      <c r="AP4" s="51"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="34" t="s">
+      <c r="AR4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="35"/>
+      <c r="AS4" s="51"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="34" t="s">
+      <c r="AU4" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="35"/>
+      <c r="AV4" s="51"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="34" t="s">
+      <c r="AX4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="35"/>
-      <c r="AZ4" s="34" t="s">
+      <c r="AY4" s="51"/>
+      <c r="AZ4" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="35"/>
+      <c r="BA4" s="51"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1366,7 +1368,7 @@
       <c r="BA6" s="17"/>
     </row>
     <row r="7" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="24"/>
       <c r="D7" s="19" t="s">
         <v>56</v>
@@ -1489,8 +1491,8 @@
       <c r="C8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="22"/>
       <c r="G8" s="29"/>
       <c r="H8" s="15"/>
@@ -3064,9 +3066,9 @@
       <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="30"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
@@ -3116,9 +3118,9 @@
       <c r="BA26" s="17"/>
     </row>
     <row r="27" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46" t="s">
+      <c r="B27" s="41"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="23" t="s">
@@ -3237,9 +3239,9 @@
       <c r="C28" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="29"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -3289,8 +3291,8 @@
       <c r="BA28" s="17"/>
     </row>
     <row r="29" spans="2:53" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="45"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="19" t="s">
         <v>56</v>
       </c>
@@ -3412,9 +3414,9 @@
       <c r="C30" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="29"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
@@ -3464,7 +3466,7 @@
       <c r="BA30" s="17"/>
     </row>
     <row r="31" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="24"/>
       <c r="D31" s="19" t="s">
         <v>56</v>
@@ -3587,9 +3589,9 @@
       <c r="C32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="29"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -3760,7 +3762,7 @@
       <c r="C34" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="44"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="21"/>
       <c r="F34" s="12"/>
       <c r="G34" s="29"/>
@@ -3927,7 +3929,7 @@
       </c>
     </row>
     <row r="36" spans="2:53" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="24" t="s">
         <v>74</v>
       </c>
@@ -4098,7 +4100,7 @@
       </c>
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B38" s="43"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="24" t="s">
         <v>77</v>
       </c>
@@ -4269,7 +4271,7 @@
       </c>
     </row>
     <row r="40" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B40" s="43"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="24" t="s">
         <v>79</v>
       </c>
@@ -4672,10 +4674,10 @@
       <c r="D45" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E45" s="44" t="s">
+      <c r="E45" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="44" t="s">
+      <c r="F45" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G45" s="29">
@@ -5014,10 +5016,10 @@
       <c r="D49" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="44" t="s">
+      <c r="E49" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F49" s="44" t="s">
+      <c r="F49" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G49" s="29">
@@ -5353,7 +5355,7 @@
     <row r="53" spans="2:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="29"/>
       <c r="C53" s="19"/>
-      <c r="D53" s="47" t="s">
+      <c r="D53" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E53" s="15" t="s">
@@ -5521,7 +5523,7 @@
     <row r="55" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="29"/>
       <c r="C55" s="19"/>
-      <c r="D55" s="47" t="s">
+      <c r="D55" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E55" s="15" t="s">
@@ -5692,7 +5694,7 @@
     <row r="57" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="29"/>
       <c r="C57" s="19"/>
-      <c r="D57" s="47" t="s">
+      <c r="D57" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E57" s="15" t="s">
@@ -5863,14 +5865,14 @@
     <row r="59" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="29"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="47" t="s">
+      <c r="D59" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>76</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G59" s="29">
         <v>2.5</v>
@@ -5899,78 +5901,80 @@
         <v>2.5</v>
       </c>
       <c r="S59" s="16"/>
-      <c r="T59" s="15"/>
+      <c r="T59" s="15">
+        <v>0.5</v>
+      </c>
       <c r="U59" s="15">
         <f t="shared" ref="U59" si="306">R59-T59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V59" s="16"/>
       <c r="W59" s="15"/>
       <c r="X59" s="15">
         <f t="shared" ref="X59" si="307">U59-W59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="Y59" s="16"/>
       <c r="Z59" s="15"/>
       <c r="AA59" s="15">
         <f t="shared" ref="AA59" si="308">X59-Z59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AB59" s="16"/>
       <c r="AC59" s="15"/>
       <c r="AD59" s="15">
         <f t="shared" ref="AD59" si="309">AA59-AC59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AE59" s="16"/>
       <c r="AF59" s="15"/>
       <c r="AG59" s="15">
         <f t="shared" ref="AG59" si="310">AD59-AF59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AH59" s="16"/>
       <c r="AI59" s="15"/>
       <c r="AJ59" s="15">
         <f t="shared" ref="AJ59" si="311">AG59-AI59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AK59" s="16"/>
       <c r="AL59" s="15"/>
       <c r="AM59" s="15">
         <f t="shared" ref="AM59" si="312">AJ59-AL59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AN59" s="16"/>
       <c r="AO59" s="15"/>
       <c r="AP59" s="15">
         <f t="shared" ref="AP59" si="313">AM59-AO59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AQ59" s="16"/>
       <c r="AR59" s="15"/>
       <c r="AS59" s="15">
         <f t="shared" ref="AS59" si="314">AP59-AR59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AT59" s="16"/>
       <c r="AU59" s="15"/>
       <c r="AV59" s="15">
         <f t="shared" ref="AV59" si="315">AS59-AU59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AW59" s="16"/>
       <c r="AX59" s="15"/>
       <c r="AY59" s="15">
         <f t="shared" ref="AY59" si="316">AV59-AX59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AZ59" s="17">
         <f>H59+K59+N59+Q59+T59+W59+Z59+AC59+AF59+AI59+AL59+AO59+AR59+AU59+AX59</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA59" s="17">
         <f>G59-AZ59</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="2:53" x14ac:dyDescent="0.25">
@@ -6034,14 +6038,14 @@
     <row r="61" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="29"/>
       <c r="C61" s="12"/>
-      <c r="D61" s="47" t="s">
+      <c r="D61" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E61" s="15" t="s">
         <v>76</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G61" s="29">
         <v>2.5</v>
@@ -6070,85 +6074,87 @@
         <v>2.5</v>
       </c>
       <c r="S61" s="16"/>
-      <c r="T61" s="15"/>
+      <c r="T61" s="15">
+        <v>0.5</v>
+      </c>
       <c r="U61" s="15">
         <f t="shared" ref="U61:U99" si="318">R61-T61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V61" s="16"/>
       <c r="W61" s="15"/>
       <c r="X61" s="15">
         <f t="shared" ref="X61" si="319">U61-W61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="Y61" s="16"/>
       <c r="Z61" s="15"/>
       <c r="AA61" s="15">
         <f t="shared" ref="AA61" si="320">X61-Z61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AB61" s="16"/>
       <c r="AC61" s="15"/>
       <c r="AD61" s="15">
         <f t="shared" ref="AD61" si="321">AA61-AC61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AE61" s="16"/>
       <c r="AF61" s="15"/>
       <c r="AG61" s="15">
         <f t="shared" ref="AG61" si="322">AD61-AF61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AH61" s="16"/>
       <c r="AI61" s="15"/>
       <c r="AJ61" s="15">
         <f t="shared" ref="AJ61" si="323">AG61-AI61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AK61" s="16"/>
       <c r="AL61" s="15"/>
       <c r="AM61" s="15">
         <f t="shared" ref="AM61" si="324">AJ61-AL61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AN61" s="16"/>
       <c r="AO61" s="15"/>
       <c r="AP61" s="15">
         <f t="shared" ref="AP61" si="325">AM61-AO61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AQ61" s="16"/>
       <c r="AR61" s="15"/>
       <c r="AS61" s="15">
         <f t="shared" ref="AS61" si="326">AP61-AR61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AT61" s="16"/>
       <c r="AU61" s="15"/>
       <c r="AV61" s="15">
         <f t="shared" ref="AV61" si="327">AS61-AU61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AW61" s="16"/>
       <c r="AX61" s="15"/>
       <c r="AY61" s="15">
         <f t="shared" ref="AY61" si="328">AV61-AX61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AZ61" s="17">
         <f>H61+K61+N61+Q61+T61+W61+Z61+AC61+AF61+AI61+AL61+AO61+AR61+AU61+AX61</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA61" s="17">
         <f>G61-AZ61</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="2:53" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="42" t="s">
+      <c r="C62" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D62" s="19"/>
@@ -6205,14 +6211,14 @@
     <row r="63" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="29"/>
       <c r="C63" s="12"/>
-      <c r="D63" s="47" t="s">
+      <c r="D63" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E63" s="15" t="s">
         <v>76</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G63" s="29">
         <v>2.5</v>
@@ -6247,72 +6253,74 @@
         <v>2.5</v>
       </c>
       <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
+      <c r="W63" s="15">
+        <v>1</v>
+      </c>
       <c r="X63" s="15">
         <f t="shared" ref="X63:X99" si="330">U63-W63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
       <c r="AA63" s="15">
         <f t="shared" ref="AA63:AA99" si="331">X63-Z63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB63" s="15"/>
       <c r="AC63" s="15"/>
       <c r="AD63" s="15">
         <f t="shared" ref="AD63:AD99" si="332">AA63-AC63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AE63" s="15"/>
       <c r="AF63" s="15"/>
       <c r="AG63" s="15">
         <f t="shared" ref="AG63:AG99" si="333">AD63-AF63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AH63" s="15"/>
       <c r="AI63" s="15"/>
       <c r="AJ63" s="15">
         <f t="shared" ref="AJ63:AJ99" si="334">AG63-AI63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AK63" s="15"/>
       <c r="AL63" s="15"/>
       <c r="AM63" s="15">
         <f t="shared" ref="AM63:AM99" si="335">AJ63-AL63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AN63" s="15"/>
       <c r="AO63" s="15"/>
       <c r="AP63" s="15">
         <f t="shared" ref="AP63:AP99" si="336">AM63-AO63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
       <c r="AS63" s="15">
         <f t="shared" ref="AS63:AS99" si="337">AP63-AR63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AT63" s="15"/>
       <c r="AU63" s="15"/>
       <c r="AV63" s="15">
         <f t="shared" ref="AV63:AV99" si="338">AS63-AU63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AW63" s="15"/>
       <c r="AX63" s="15"/>
       <c r="AY63" s="15">
         <f t="shared" ref="AY63:AY99" si="339">AV63-AX63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AZ63" s="17">
         <f t="shared" ref="AZ63:AZ99" si="340">H63+K63+N63+Q63+T63+W63+Z63+AC63+AF63+AI63+AL63+AO63+AR63+AU63+AX63</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA63" s="17">
         <f t="shared" ref="BA63:BA99" si="341">G63-AZ63</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="64" spans="2:53" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6322,10 +6330,10 @@
       <c r="C64" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="48"/>
+      <c r="D64" s="46"/>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="49"/>
+      <c r="G64" s="47"/>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
       <c r="J64" s="16"/>
@@ -6376,14 +6384,14 @@
     <row r="65" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="29"/>
       <c r="C65" s="19"/>
-      <c r="D65" s="47" t="s">
+      <c r="D65" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E65" s="15" t="s">
         <v>76</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G65" s="29">
         <v>2.5</v>
@@ -6418,72 +6426,74 @@
         <v>2.5</v>
       </c>
       <c r="V65" s="16"/>
-      <c r="W65" s="15"/>
+      <c r="W65" s="15">
+        <v>1</v>
+      </c>
       <c r="X65" s="15">
         <f t="shared" si="330"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="Y65" s="16"/>
       <c r="Z65" s="15"/>
       <c r="AA65" s="15">
         <f t="shared" si="331"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB65" s="16"/>
       <c r="AC65" s="15"/>
       <c r="AD65" s="15">
         <f t="shared" si="332"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AE65" s="16"/>
       <c r="AF65" s="15"/>
       <c r="AG65" s="15">
         <f t="shared" si="333"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AH65" s="16"/>
       <c r="AI65" s="15"/>
       <c r="AJ65" s="15">
         <f t="shared" si="334"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AK65" s="16"/>
       <c r="AL65" s="15"/>
       <c r="AM65" s="15">
         <f t="shared" si="335"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AN65" s="16"/>
       <c r="AO65" s="15"/>
       <c r="AP65" s="15">
         <f t="shared" si="336"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AQ65" s="16"/>
       <c r="AR65" s="15"/>
       <c r="AS65" s="15">
         <f t="shared" si="337"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AT65" s="16"/>
       <c r="AU65" s="15"/>
       <c r="AV65" s="15">
         <f t="shared" si="338"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AW65" s="16"/>
       <c r="AX65" s="15"/>
       <c r="AY65" s="15">
         <f t="shared" si="339"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AZ65" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA65" s="17">
         <f t="shared" si="341"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="66" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
@@ -6545,7 +6555,7 @@
       <c r="BA66" s="17"/>
     </row>
     <row r="67" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B67" s="50"/>
+      <c r="B67" s="48"/>
       <c r="C67" s="19"/>
       <c r="D67" s="22" t="s">
         <v>98</v>
@@ -6716,7 +6726,7 @@
       <c r="BA68" s="17"/>
     </row>
     <row r="69" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B69" s="50"/>
+      <c r="B69" s="48"/>
       <c r="C69" s="19"/>
       <c r="D69" s="22" t="s">
         <v>98</v>
@@ -6887,7 +6897,7 @@
       <c r="BA70" s="17"/>
     </row>
     <row r="71" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B71" s="50"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="19"/>
       <c r="D71" s="22" t="s">
         <v>98</v>
@@ -7058,7 +7068,7 @@
       <c r="BA72" s="17"/>
     </row>
     <row r="73" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B73" s="50"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="19"/>
       <c r="D73" s="22" t="s">
         <v>98</v>
@@ -7229,7 +7239,7 @@
       <c r="BA74" s="17"/>
     </row>
     <row r="75" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="50"/>
+      <c r="B75" s="48"/>
       <c r="C75" s="19"/>
       <c r="D75" s="22" t="s">
         <v>98</v>
@@ -7400,7 +7410,7 @@
       <c r="BA76" s="17"/>
     </row>
     <row r="77" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="50"/>
+      <c r="B77" s="48"/>
       <c r="C77" s="19"/>
       <c r="D77" s="22" t="s">
         <v>98</v>
@@ -7569,7 +7579,7 @@
       <c r="BA78" s="17"/>
     </row>
     <row r="79" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="50"/>
+      <c r="B79" s="48"/>
       <c r="C79" s="19"/>
       <c r="D79" s="22" t="s">
         <v>98</v>
@@ -7738,7 +7748,7 @@
       <c r="BA80" s="17"/>
     </row>
     <row r="81" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="50"/>
+      <c r="B81" s="48"/>
       <c r="C81" s="19"/>
       <c r="D81" s="22" t="s">
         <v>98</v>
@@ -7907,7 +7917,7 @@
       <c r="BA82" s="17"/>
     </row>
     <row r="83" spans="2:53" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="50"/>
+      <c r="B83" s="48"/>
       <c r="C83" s="19"/>
       <c r="D83" s="22" t="s">
         <v>98</v>
@@ -8075,7 +8085,7 @@
       <c r="BA84" s="17"/>
     </row>
     <row r="85" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B85" s="50"/>
+      <c r="B85" s="48"/>
       <c r="C85" s="19"/>
       <c r="D85" s="22" t="s">
         <v>98</v>
@@ -8189,7 +8199,7 @@
       <c r="B86" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="42" t="s">
+      <c r="C86" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D86" s="13"/>
@@ -8244,7 +8254,7 @@
       <c r="BA86" s="17"/>
     </row>
     <row r="87" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B87" s="50"/>
+      <c r="B87" s="48"/>
       <c r="C87" s="19"/>
       <c r="D87" s="22" t="s">
         <v>98</v>
@@ -8748,8 +8758,8 @@
     </row>
     <row r="93" spans="2:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="20"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="47" t="s">
+      <c r="C93" s="49"/>
+      <c r="D93" s="45" t="s">
         <v>102</v>
       </c>
       <c r="E93" s="15" t="s">
@@ -9335,60 +9345,65 @@
       </c>
     </row>
     <row r="100" spans="2:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="36"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="38"/>
+      <c r="C100" s="34"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="36"/>
       <c r="F100" s="25"/>
-      <c r="G100" s="39"/>
+      <c r="G100" s="37"/>
       <c r="H100" s="25"/>
       <c r="I100" s="25"/>
-      <c r="J100" s="40"/>
+      <c r="J100" s="38"/>
       <c r="K100" s="25"/>
       <c r="L100" s="25"/>
-      <c r="M100" s="40"/>
+      <c r="M100" s="38"/>
       <c r="N100" s="25"/>
       <c r="O100" s="25"/>
-      <c r="P100" s="40"/>
+      <c r="P100" s="38"/>
       <c r="Q100" s="25"/>
       <c r="R100" s="25"/>
-      <c r="S100" s="40"/>
+      <c r="S100" s="38"/>
       <c r="T100" s="25"/>
       <c r="U100" s="25"/>
-      <c r="V100" s="40"/>
+      <c r="V100" s="38"/>
       <c r="W100" s="25"/>
       <c r="X100" s="25"/>
-      <c r="Y100" s="40"/>
+      <c r="Y100" s="38"/>
       <c r="Z100" s="25"/>
       <c r="AA100" s="25"/>
-      <c r="AB100" s="40"/>
+      <c r="AB100" s="38"/>
       <c r="AC100" s="25"/>
       <c r="AD100" s="25"/>
-      <c r="AE100" s="40"/>
+      <c r="AE100" s="38"/>
       <c r="AF100" s="25"/>
       <c r="AG100" s="25"/>
-      <c r="AH100" s="40"/>
+      <c r="AH100" s="38"/>
       <c r="AI100" s="25"/>
       <c r="AJ100" s="25"/>
-      <c r="AK100" s="40"/>
+      <c r="AK100" s="38"/>
       <c r="AL100" s="25"/>
       <c r="AM100" s="25"/>
-      <c r="AN100" s="40"/>
+      <c r="AN100" s="38"/>
       <c r="AO100" s="25"/>
       <c r="AP100" s="25"/>
-      <c r="AQ100" s="40"/>
+      <c r="AQ100" s="38"/>
       <c r="AR100" s="25"/>
       <c r="AS100" s="25"/>
-      <c r="AT100" s="40"/>
+      <c r="AT100" s="38"/>
       <c r="AU100" s="25"/>
       <c r="AV100" s="25"/>
-      <c r="AW100" s="40"/>
+      <c r="AW100" s="38"/>
       <c r="AX100" s="25"/>
       <c r="AY100" s="25"/>
-      <c r="AZ100" s="41"/>
-      <c r="BA100" s="41"/>
+      <c r="AZ100" s="39"/>
+      <c r="BA100" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9400,11 +9415,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -9425,7 +9435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se añadieron los diagramas de robustez
Se añadieron los diagramas de robustez correspondientes al rubro de Grupos. También se actualizaron la plantilla de tareas y la de casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
+++ b/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A0FF5-C48E-4A52-A183-C13F3380EA20}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="105">
   <si>
     <t>Columna</t>
   </si>
@@ -349,6 +350,9 @@
   </si>
   <si>
     <t>En proceso</t>
+  </si>
+  <si>
+    <t>En Proceso</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1022,13 +1026,13 @@
   <dimension ref="B1:BA100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="S57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomRight" activeCell="AC56" sqref="AC56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -5191,7 +5195,7 @@
         <v>51</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G51" s="29">
         <v>2.5</v>
@@ -5238,60 +5242,62 @@
         <v>2.5</v>
       </c>
       <c r="AB51" s="16"/>
-      <c r="AC51" s="15"/>
+      <c r="AC51" s="15">
+        <v>0.4</v>
+      </c>
       <c r="AD51" s="15">
         <f t="shared" ref="AD51" si="262">AA51-AC51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AE51" s="16"/>
       <c r="AF51" s="15"/>
       <c r="AG51" s="15">
         <f t="shared" ref="AG51" si="263">AD51-AF51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AH51" s="16"/>
       <c r="AI51" s="15"/>
       <c r="AJ51" s="15">
         <f t="shared" ref="AJ51" si="264">AG51-AI51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AK51" s="16"/>
       <c r="AL51" s="15"/>
       <c r="AM51" s="15">
         <f t="shared" ref="AM51" si="265">AJ51-AL51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AN51" s="16"/>
       <c r="AO51" s="15"/>
       <c r="AP51" s="15">
         <f t="shared" ref="AP51" si="266">AM51-AO51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AQ51" s="16"/>
       <c r="AR51" s="15"/>
       <c r="AS51" s="15">
         <f t="shared" ref="AS51" si="267">AP51-AR51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AT51" s="16"/>
       <c r="AU51" s="15"/>
       <c r="AV51" s="15">
         <f t="shared" ref="AV51" si="268">AS51-AU51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AW51" s="16"/>
       <c r="AX51" s="15"/>
       <c r="AY51" s="15">
         <f t="shared" ref="AY51" si="269">AV51-AX51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AZ51" s="17">
         <f>H51+K51+N51+Q51+T51+W51+Z51+AC51+AF51+AI51+AL51+AO51+AR51+AU51+AX51</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="BA51" s="17">
         <f>G51-AZ51</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="52" spans="2:53" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -5362,7 +5368,7 @@
         <v>51</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="G53" s="29">
         <v>2.5</v>
@@ -5409,57 +5415,59 @@
         <v>2.5</v>
       </c>
       <c r="AB53" s="16"/>
-      <c r="AC53" s="15"/>
+      <c r="AC53" s="15">
+        <v>0.5</v>
+      </c>
       <c r="AD53" s="15">
         <f t="shared" ref="AD53" si="274">AA53-AC53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AE53" s="16"/>
       <c r="AF53" s="15"/>
       <c r="AG53" s="15">
         <f t="shared" ref="AG53" si="275">AD53-AF53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AH53" s="16"/>
       <c r="AI53" s="15"/>
       <c r="AJ53" s="15">
         <f t="shared" ref="AJ53" si="276">AG53-AI53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AK53" s="16"/>
       <c r="AL53" s="15"/>
       <c r="AM53" s="15">
         <f t="shared" ref="AM53" si="277">AJ53-AL53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AN53" s="16"/>
       <c r="AO53" s="15"/>
       <c r="AP53" s="15">
         <f t="shared" ref="AP53" si="278">AM53-AO53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AQ53" s="16"/>
       <c r="AR53" s="15"/>
       <c r="AS53" s="15">
         <f t="shared" ref="AS53" si="279">AP53-AR53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AT53" s="16"/>
       <c r="AU53" s="15"/>
       <c r="AV53" s="15">
         <f t="shared" ref="AV53" si="280">AS53-AU53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AW53" s="16"/>
       <c r="AX53" s="15"/>
       <c r="AY53" s="15"/>
       <c r="AZ53" s="17">
         <f>H53+K53+N53+Q53+T53+W53+Z53+AC53+AF53+AI53+AL53+AO53+AR53+AU53+AX53</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA53" s="17">
         <f>G53-AZ53</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="2:53" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5530,7 +5538,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G55" s="29">
         <v>2.5</v>
@@ -5577,60 +5585,62 @@
         <v>2.5</v>
       </c>
       <c r="AB55" s="16"/>
-      <c r="AC55" s="15"/>
+      <c r="AC55" s="15">
+        <v>0.4</v>
+      </c>
       <c r="AD55" s="15">
         <f t="shared" ref="AD55" si="285">AA55-AC55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AE55" s="16"/>
       <c r="AF55" s="15"/>
       <c r="AG55" s="15">
         <f t="shared" ref="AG55" si="286">AD55-AF55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AH55" s="16"/>
       <c r="AI55" s="15"/>
       <c r="AJ55" s="15">
         <f t="shared" ref="AJ55" si="287">AG55-AI55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AK55" s="16"/>
       <c r="AL55" s="15"/>
       <c r="AM55" s="15">
         <f t="shared" ref="AM55" si="288">AJ55-AL55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AN55" s="16"/>
       <c r="AO55" s="15"/>
       <c r="AP55" s="15">
         <f t="shared" ref="AP55" si="289">AM55-AO55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AQ55" s="16"/>
       <c r="AR55" s="15"/>
       <c r="AS55" s="15">
         <f t="shared" ref="AS55" si="290">AP55-AR55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AT55" s="16"/>
       <c r="AU55" s="15"/>
       <c r="AV55" s="15">
         <f t="shared" ref="AV55" si="291">AS55-AU55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AW55" s="16"/>
       <c r="AX55" s="15"/>
       <c r="AY55" s="15">
         <f t="shared" ref="AY55" si="292">AV55-AX55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="AZ55" s="17">
         <f>H55+K55+N55+Q55+T55+W55+Z55+AC55+AF55+AI55+AL55+AO55+AR55+AU55+AX55</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="BA55" s="17">
         <f>G55-AZ55</f>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="56" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
@@ -5701,7 +5711,7 @@
         <v>51</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="G57" s="29">
         <v>2.5</v>
@@ -5742,66 +5752,70 @@
         <v>2.5</v>
       </c>
       <c r="Y57" s="16"/>
-      <c r="Z57" s="15"/>
+      <c r="Z57" s="15">
+        <v>1</v>
+      </c>
       <c r="AA57" s="15">
         <f t="shared" ref="AA57" si="296">X57-Z57</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB57" s="16"/>
-      <c r="AC57" s="15"/>
+      <c r="AC57" s="15">
+        <v>0.5</v>
+      </c>
       <c r="AD57" s="15">
         <f t="shared" ref="AD57" si="297">AA57-AC57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AE57" s="16"/>
       <c r="AF57" s="15"/>
       <c r="AG57" s="15">
         <f t="shared" ref="AG57" si="298">AD57-AF57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AH57" s="16"/>
       <c r="AI57" s="15"/>
       <c r="AJ57" s="15">
         <f t="shared" ref="AJ57" si="299">AG57-AI57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AK57" s="16"/>
       <c r="AL57" s="15"/>
       <c r="AM57" s="15">
         <f t="shared" ref="AM57" si="300">AJ57-AL57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AN57" s="16"/>
       <c r="AO57" s="15"/>
       <c r="AP57" s="15">
         <f t="shared" ref="AP57" si="301">AM57-AO57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AQ57" s="16"/>
       <c r="AR57" s="15"/>
       <c r="AS57" s="15">
         <f t="shared" ref="AS57" si="302">AP57-AR57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AT57" s="16"/>
       <c r="AU57" s="15"/>
       <c r="AV57" s="15">
         <f t="shared" ref="AV57" si="303">AS57-AU57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AW57" s="16"/>
       <c r="AX57" s="15"/>
       <c r="AY57" s="15">
         <f t="shared" ref="AY57" si="304">AV57-AX57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AZ57" s="17">
         <f>H57+K57+N57+Q57+T57+W57+Z57+AC57+AF57+AI57+AL57+AO57+AR57+AU57+AX57</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA57" s="17">
         <f>G57-AZ57</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:53" x14ac:dyDescent="0.25">
@@ -9399,11 +9413,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9415,6 +9424,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -9439,7 +9453,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Diagramas de secuencia y registros de tiempo
Se agregaron los diagramas de secuencia de los CU 14,15,16,21, así mismo se registraron los tiempos que se invirtieron en realizarlos.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
+++ b/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C12F51B-307F-4E93-9736-B85DBD066333}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668AE671-2173-4B99-A892-EA2283927C0F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,18 +1031,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA100"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AG41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="5" topLeftCell="AR58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="59" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
@@ -5910,7 +5910,7 @@
         <v>76</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G59" s="29">
         <v>2.5</v>
@@ -5940,79 +5940,80 @@
       </c>
       <c r="S59" s="16"/>
       <c r="T59" s="15">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="U59" s="15">
         <f t="shared" ref="U59" si="306">R59-T59</f>
-        <v>2</v>
+        <v>1.92</v>
       </c>
       <c r="V59" s="16"/>
       <c r="W59" s="15"/>
       <c r="X59" s="15">
         <f t="shared" ref="X59" si="307">U59-W59</f>
-        <v>2</v>
+        <v>1.92</v>
       </c>
       <c r="Y59" s="16"/>
-      <c r="Z59" s="15"/>
+      <c r="Z59" s="15">
+        <v>1</v>
+      </c>
       <c r="AA59" s="15">
-        <f t="shared" ref="AA59" si="308">X59-Z59</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AB59" s="16"/>
       <c r="AC59" s="15"/>
       <c r="AD59" s="15">
-        <f t="shared" ref="AD59" si="309">AA59-AC59</f>
-        <v>2</v>
+        <f t="shared" ref="AD59" si="308">AA59-AC59</f>
+        <v>0.5</v>
       </c>
       <c r="AE59" s="16"/>
       <c r="AF59" s="15"/>
       <c r="AG59" s="15">
-        <f t="shared" ref="AG59" si="310">AD59-AF59</f>
-        <v>2</v>
+        <f t="shared" ref="AG59" si="309">AD59-AF59</f>
+        <v>0.5</v>
       </c>
       <c r="AH59" s="16"/>
       <c r="AI59" s="15"/>
       <c r="AJ59" s="15">
-        <f t="shared" ref="AJ59" si="311">AG59-AI59</f>
-        <v>2</v>
+        <f t="shared" ref="AJ59" si="310">AG59-AI59</f>
+        <v>0.5</v>
       </c>
       <c r="AK59" s="16"/>
       <c r="AL59" s="15"/>
       <c r="AM59" s="15">
-        <f t="shared" ref="AM59" si="312">AJ59-AL59</f>
-        <v>2</v>
+        <f t="shared" ref="AM59" si="311">AJ59-AL59</f>
+        <v>0.5</v>
       </c>
       <c r="AN59" s="16"/>
       <c r="AO59" s="15"/>
       <c r="AP59" s="15">
-        <f t="shared" ref="AP59" si="313">AM59-AO59</f>
-        <v>2</v>
+        <f t="shared" ref="AP59" si="312">AM59-AO59</f>
+        <v>0.5</v>
       </c>
       <c r="AQ59" s="16"/>
       <c r="AR59" s="15"/>
       <c r="AS59" s="15">
-        <f t="shared" ref="AS59" si="314">AP59-AR59</f>
-        <v>2</v>
+        <f t="shared" ref="AS59" si="313">AP59-AR59</f>
+        <v>0.5</v>
       </c>
       <c r="AT59" s="16"/>
       <c r="AU59" s="15"/>
       <c r="AV59" s="15">
-        <f t="shared" ref="AV59" si="315">AS59-AU59</f>
-        <v>2</v>
+        <f t="shared" ref="AV59" si="314">AS59-AU59</f>
+        <v>0.5</v>
       </c>
       <c r="AW59" s="16"/>
       <c r="AX59" s="15"/>
       <c r="AY59" s="15">
-        <f t="shared" ref="AY59" si="316">AV59-AX59</f>
-        <v>2</v>
+        <f t="shared" ref="AY59" si="315">AV59-AX59</f>
+        <v>0.5</v>
       </c>
       <c r="AZ59" s="17">
         <f>H59+K59+N59+Q59+T59+W59+Z59+AC59+AF59+AI59+AL59+AO59+AR59+AU59+AX59</f>
-        <v>0.5</v>
+        <v>1.58</v>
       </c>
       <c r="BA59" s="17">
         <f>G59-AZ59</f>
-        <v>2</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="60" spans="2:53" x14ac:dyDescent="0.25">
@@ -6083,7 +6084,7 @@
         <v>76</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G61" s="29">
         <v>2.5</v>
@@ -6108,84 +6109,86 @@
       <c r="P61" s="15"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15">
-        <f t="shared" ref="R61:R99" si="317">O61-Q61</f>
+        <f t="shared" ref="R61:R99" si="316">O61-Q61</f>
         <v>2.5</v>
       </c>
       <c r="S61" s="16"/>
       <c r="T61" s="15">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="U61" s="15">
-        <f t="shared" ref="U61:U99" si="318">R61-T61</f>
-        <v>2</v>
+        <f t="shared" ref="U61:U99" si="317">R61-T61</f>
+        <v>1.92</v>
       </c>
       <c r="V61" s="16"/>
       <c r="W61" s="15"/>
       <c r="X61" s="15">
-        <f t="shared" ref="X61" si="319">U61-W61</f>
-        <v>2</v>
+        <f t="shared" ref="X61" si="318">U61-W61</f>
+        <v>1.92</v>
       </c>
       <c r="Y61" s="16"/>
-      <c r="Z61" s="15"/>
+      <c r="Z61" s="15">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="AA61" s="15">
-        <f t="shared" ref="AA61" si="320">X61-Z61</f>
-        <v>2</v>
+        <f t="shared" ref="AA61" si="319">X61-Z61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AB61" s="16"/>
       <c r="AC61" s="15"/>
       <c r="AD61" s="15">
-        <f t="shared" ref="AD61" si="321">AA61-AC61</f>
-        <v>2</v>
+        <f t="shared" ref="AD61" si="320">AA61-AC61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AE61" s="16"/>
       <c r="AF61" s="15"/>
       <c r="AG61" s="15">
-        <f t="shared" ref="AG61" si="322">AD61-AF61</f>
-        <v>2</v>
+        <f t="shared" ref="AG61" si="321">AD61-AF61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AH61" s="16"/>
       <c r="AI61" s="15"/>
       <c r="AJ61" s="15">
-        <f t="shared" ref="AJ61" si="323">AG61-AI61</f>
-        <v>2</v>
+        <f t="shared" ref="AJ61" si="322">AG61-AI61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AK61" s="16"/>
       <c r="AL61" s="15"/>
       <c r="AM61" s="15">
-        <f t="shared" ref="AM61" si="324">AJ61-AL61</f>
-        <v>2</v>
+        <f t="shared" ref="AM61" si="323">AJ61-AL61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AN61" s="16"/>
       <c r="AO61" s="15"/>
       <c r="AP61" s="15">
-        <f t="shared" ref="AP61" si="325">AM61-AO61</f>
-        <v>2</v>
+        <f t="shared" ref="AP61" si="324">AM61-AO61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AQ61" s="16"/>
       <c r="AR61" s="15"/>
       <c r="AS61" s="15">
-        <f t="shared" ref="AS61" si="326">AP61-AR61</f>
-        <v>2</v>
+        <f t="shared" ref="AS61" si="325">AP61-AR61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AT61" s="16"/>
       <c r="AU61" s="15"/>
       <c r="AV61" s="15">
-        <f t="shared" ref="AV61" si="327">AS61-AU61</f>
-        <v>2</v>
+        <f t="shared" ref="AV61" si="326">AS61-AU61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AW61" s="16"/>
       <c r="AX61" s="15"/>
       <c r="AY61" s="15">
-        <f t="shared" ref="AY61" si="328">AV61-AX61</f>
-        <v>2</v>
+        <f t="shared" ref="AY61" si="327">AV61-AX61</f>
+        <v>1.3399999999999999</v>
       </c>
       <c r="AZ61" s="17">
         <f>H61+K61+N61+Q61+T61+W61+Z61+AC61+AF61+AI61+AL61+AO61+AR61+AU61+AX61</f>
-        <v>0.5</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="BA61" s="17">
         <f>G61-AZ61</f>
-        <v>2</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="62" spans="2:53" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6256,14 +6259,14 @@
         <v>76</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G63" s="29">
         <v>2.5</v>
       </c>
       <c r="H63" s="15"/>
       <c r="I63" s="15">
-        <f t="shared" ref="I63:I99" si="329">G63-H63</f>
+        <f t="shared" ref="I63:I99" si="328">G63-H63</f>
         <v>2.5</v>
       </c>
       <c r="J63" s="16"/>
@@ -6281,13 +6284,13 @@
       <c r="P63" s="16"/>
       <c r="Q63" s="15"/>
       <c r="R63" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2.5</v>
       </c>
       <c r="S63" s="16"/>
       <c r="T63" s="15"/>
       <c r="U63" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2.5</v>
       </c>
       <c r="V63" s="15"/>
@@ -6295,70 +6298,72 @@
         <v>1</v>
       </c>
       <c r="X63" s="15">
-        <f t="shared" ref="X63:X99" si="330">U63-W63</f>
+        <f t="shared" ref="X63:X99" si="329">U63-W63</f>
         <v>1.5</v>
       </c>
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
       <c r="AA63" s="15">
-        <f t="shared" ref="AA63:AA99" si="331">X63-Z63</f>
+        <f t="shared" ref="AA63:AA99" si="330">X63-Z63</f>
         <v>1.5</v>
       </c>
       <c r="AB63" s="15"/>
-      <c r="AC63" s="15"/>
+      <c r="AC63" s="15">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="AD63" s="15">
-        <f t="shared" ref="AD63:AD99" si="332">AA63-AC63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AD63:AD99" si="331">AA63-AC63</f>
+        <v>0.92</v>
       </c>
       <c r="AE63" s="15"/>
       <c r="AF63" s="15"/>
       <c r="AG63" s="15">
-        <f t="shared" ref="AG63:AG99" si="333">AD63-AF63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AG63:AG99" si="332">AD63-AF63</f>
+        <v>0.92</v>
       </c>
       <c r="AH63" s="15"/>
       <c r="AI63" s="15"/>
       <c r="AJ63" s="15">
-        <f t="shared" ref="AJ63:AJ99" si="334">AG63-AI63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AJ63:AJ99" si="333">AG63-AI63</f>
+        <v>0.92</v>
       </c>
       <c r="AK63" s="15"/>
       <c r="AL63" s="15"/>
       <c r="AM63" s="15">
-        <f t="shared" ref="AM63:AM99" si="335">AJ63-AL63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AM63:AM99" si="334">AJ63-AL63</f>
+        <v>0.92</v>
       </c>
       <c r="AN63" s="15"/>
       <c r="AO63" s="15"/>
       <c r="AP63" s="15">
-        <f t="shared" ref="AP63:AP99" si="336">AM63-AO63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AP63:AP99" si="335">AM63-AO63</f>
+        <v>0.92</v>
       </c>
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
       <c r="AS63" s="15">
-        <f t="shared" ref="AS63:AS99" si="337">AP63-AR63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AS63:AS99" si="336">AP63-AR63</f>
+        <v>0.92</v>
       </c>
       <c r="AT63" s="15"/>
       <c r="AU63" s="15"/>
       <c r="AV63" s="15">
-        <f t="shared" ref="AV63:AV99" si="338">AS63-AU63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AV63:AV99" si="337">AS63-AU63</f>
+        <v>0.92</v>
       </c>
       <c r="AW63" s="15"/>
       <c r="AX63" s="15"/>
       <c r="AY63" s="15">
-        <f t="shared" ref="AY63:AY99" si="339">AV63-AX63</f>
-        <v>1.5</v>
+        <f t="shared" ref="AY63:AY99" si="338">AV63-AX63</f>
+        <v>0.92</v>
       </c>
       <c r="AZ63" s="17">
-        <f t="shared" ref="AZ63:AZ99" si="340">H63+K63+N63+Q63+T63+W63+Z63+AC63+AF63+AI63+AL63+AO63+AR63+AU63+AX63</f>
-        <v>1</v>
+        <f t="shared" ref="AZ63:AZ99" si="339">H63+K63+N63+Q63+T63+W63+Z63+AC63+AF63+AI63+AL63+AO63+AR63+AU63+AX63</f>
+        <v>1.58</v>
       </c>
       <c r="BA63" s="17">
-        <f t="shared" ref="BA63:BA99" si="341">G63-AZ63</f>
-        <v>1.5</v>
+        <f t="shared" ref="BA63:BA99" si="340">G63-AZ63</f>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="64" spans="2:53" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6429,14 +6434,14 @@
         <v>76</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G65" s="29">
         <v>2.5</v>
       </c>
       <c r="H65" s="15"/>
       <c r="I65" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2.5</v>
       </c>
       <c r="J65" s="16"/>
@@ -6454,13 +6459,13 @@
       <c r="P65" s="16"/>
       <c r="Q65" s="15"/>
       <c r="R65" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2.5</v>
       </c>
       <c r="S65" s="16"/>
       <c r="T65" s="15"/>
       <c r="U65" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2.5</v>
       </c>
       <c r="V65" s="16"/>
@@ -6468,73 +6473,75 @@
         <v>1</v>
       </c>
       <c r="X65" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>1.5</v>
       </c>
       <c r="Y65" s="16"/>
       <c r="Z65" s="15"/>
       <c r="AA65" s="15">
+        <f t="shared" si="330"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB65" s="16"/>
+      <c r="AC65" s="15">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AD65" s="15">
         <f t="shared" si="331"/>
-        <v>1.5</v>
-      </c>
-      <c r="AB65" s="16"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15">
-        <f t="shared" si="332"/>
-        <v>1.5</v>
+        <v>0.92</v>
       </c>
       <c r="AE65" s="16"/>
       <c r="AF65" s="15"/>
       <c r="AG65" s="15">
-        <f t="shared" si="333"/>
-        <v>1.5</v>
+        <f t="shared" si="332"/>
+        <v>0.92</v>
       </c>
       <c r="AH65" s="16"/>
       <c r="AI65" s="15"/>
       <c r="AJ65" s="15">
-        <f t="shared" si="334"/>
-        <v>1.5</v>
+        <f t="shared" si="333"/>
+        <v>0.92</v>
       </c>
       <c r="AK65" s="16"/>
       <c r="AL65" s="15"/>
       <c r="AM65" s="15">
-        <f t="shared" si="335"/>
-        <v>1.5</v>
+        <f t="shared" si="334"/>
+        <v>0.92</v>
       </c>
       <c r="AN65" s="16"/>
       <c r="AO65" s="15"/>
       <c r="AP65" s="15">
-        <f t="shared" si="336"/>
-        <v>1.5</v>
+        <f t="shared" si="335"/>
+        <v>0.92</v>
       </c>
       <c r="AQ65" s="16"/>
       <c r="AR65" s="15"/>
       <c r="AS65" s="15">
-        <f t="shared" si="337"/>
-        <v>1.5</v>
+        <f t="shared" si="336"/>
+        <v>0.92</v>
       </c>
       <c r="AT65" s="16"/>
       <c r="AU65" s="15"/>
       <c r="AV65" s="15">
-        <f t="shared" si="338"/>
-        <v>1.5</v>
+        <f t="shared" si="337"/>
+        <v>0.92</v>
       </c>
       <c r="AW65" s="16"/>
       <c r="AX65" s="15"/>
       <c r="AY65" s="15">
+        <f t="shared" si="338"/>
+        <v>0.92</v>
+      </c>
+      <c r="AZ65" s="17">
         <f t="shared" si="339"/>
-        <v>1.5</v>
-      </c>
-      <c r="AZ65" s="17">
+        <v>1.58</v>
+      </c>
+      <c r="BA65" s="17">
         <f t="shared" si="340"/>
-        <v>1</v>
-      </c>
-      <c r="BA65" s="17">
-        <f t="shared" si="341"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+        <v>0.91999999999999993</v>
+      </c>
+    </row>
+    <row r="66" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B66" s="29" t="s">
         <v>83</v>
       </c>
@@ -6609,7 +6616,7 @@
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J67" s="16"/>
@@ -6627,81 +6634,81 @@
       <c r="P67" s="16"/>
       <c r="Q67" s="15"/>
       <c r="R67" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S67" s="16"/>
       <c r="T67" s="15"/>
       <c r="U67" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V67" s="15"/>
       <c r="W67" s="15"/>
       <c r="X67" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y67" s="15"/>
       <c r="Z67" s="15"/>
       <c r="AA67" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB67" s="15"/>
       <c r="AC67" s="15"/>
       <c r="AD67" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE67" s="15"/>
       <c r="AF67" s="15"/>
       <c r="AG67" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH67" s="15"/>
       <c r="AI67" s="15"/>
       <c r="AJ67" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK67" s="15"/>
       <c r="AL67" s="15"/>
       <c r="AM67" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN67" s="15"/>
       <c r="AO67" s="15"/>
       <c r="AP67" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ67" s="15"/>
       <c r="AR67" s="15"/>
       <c r="AS67" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT67" s="15"/>
       <c r="AU67" s="15"/>
       <c r="AV67" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW67" s="15"/>
       <c r="AX67" s="15"/>
       <c r="AY67" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ67" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ67" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA67" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA67" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -6780,7 +6787,7 @@
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J69" s="16"/>
@@ -6798,81 +6805,81 @@
       <c r="P69" s="16"/>
       <c r="Q69" s="15"/>
       <c r="R69" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S69" s="16"/>
       <c r="T69" s="15"/>
       <c r="U69" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V69" s="16"/>
       <c r="W69" s="15"/>
       <c r="X69" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y69" s="16"/>
       <c r="Z69" s="15"/>
       <c r="AA69" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB69" s="16"/>
       <c r="AC69" s="15"/>
       <c r="AD69" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE69" s="16"/>
       <c r="AF69" s="15"/>
       <c r="AG69" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH69" s="16"/>
       <c r="AI69" s="15"/>
       <c r="AJ69" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK69" s="16"/>
       <c r="AL69" s="15"/>
       <c r="AM69" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN69" s="16"/>
       <c r="AO69" s="15"/>
       <c r="AP69" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ69" s="16"/>
       <c r="AR69" s="15"/>
       <c r="AS69" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT69" s="16"/>
       <c r="AU69" s="15"/>
       <c r="AV69" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW69" s="16"/>
       <c r="AX69" s="15"/>
       <c r="AY69" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ69" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ69" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA69" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA69" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -6951,7 +6958,7 @@
       </c>
       <c r="H71" s="15"/>
       <c r="I71" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J71" s="16"/>
@@ -6969,81 +6976,81 @@
       <c r="P71" s="16"/>
       <c r="Q71" s="15"/>
       <c r="R71" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S71" s="16"/>
       <c r="T71" s="15"/>
       <c r="U71" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V71" s="16"/>
       <c r="W71" s="15"/>
       <c r="X71" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y71" s="16"/>
       <c r="Z71" s="15"/>
       <c r="AA71" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB71" s="16"/>
       <c r="AC71" s="15"/>
       <c r="AD71" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE71" s="16"/>
       <c r="AF71" s="15"/>
       <c r="AG71" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH71" s="16"/>
       <c r="AI71" s="15"/>
       <c r="AJ71" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK71" s="16"/>
       <c r="AL71" s="15"/>
       <c r="AM71" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN71" s="16"/>
       <c r="AO71" s="15"/>
       <c r="AP71" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ71" s="16"/>
       <c r="AR71" s="15"/>
       <c r="AS71" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT71" s="16"/>
       <c r="AU71" s="15"/>
       <c r="AV71" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW71" s="16"/>
       <c r="AX71" s="15"/>
       <c r="AY71" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ71" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ71" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA71" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA71" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7122,99 +7129,99 @@
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J73" s="16"/>
       <c r="K73" s="15"/>
       <c r="L73" s="15">
-        <f t="shared" ref="L73:L99" si="342">I73-K73</f>
+        <f t="shared" ref="L73:L99" si="341">I73-K73</f>
         <v>2</v>
       </c>
       <c r="M73" s="16"/>
       <c r="N73" s="15"/>
       <c r="O73" s="15">
-        <f t="shared" ref="O73:O99" si="343">L73-N73</f>
+        <f t="shared" ref="O73:O99" si="342">L73-N73</f>
         <v>2</v>
       </c>
       <c r="P73" s="16"/>
       <c r="Q73" s="15"/>
       <c r="R73" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S73" s="16"/>
       <c r="T73" s="15"/>
       <c r="U73" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V73" s="16"/>
       <c r="W73" s="15"/>
       <c r="X73" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y73" s="16"/>
       <c r="Z73" s="15"/>
       <c r="AA73" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB73" s="16"/>
       <c r="AC73" s="15"/>
       <c r="AD73" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE73" s="16"/>
       <c r="AF73" s="15"/>
       <c r="AG73" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH73" s="16"/>
       <c r="AI73" s="15"/>
       <c r="AJ73" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK73" s="16"/>
       <c r="AL73" s="15"/>
       <c r="AM73" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN73" s="16"/>
       <c r="AO73" s="15"/>
       <c r="AP73" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ73" s="16"/>
       <c r="AR73" s="15"/>
       <c r="AS73" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT73" s="16"/>
       <c r="AU73" s="15"/>
       <c r="AV73" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW73" s="16"/>
       <c r="AX73" s="15"/>
       <c r="AY73" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ73" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ73" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA73" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA73" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7293,99 +7300,99 @@
       </c>
       <c r="H75" s="15"/>
       <c r="I75" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J75" s="16"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M75" s="16"/>
       <c r="N75" s="15"/>
       <c r="O75" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P75" s="16"/>
       <c r="Q75" s="15"/>
       <c r="R75" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S75" s="16"/>
       <c r="T75" s="15"/>
       <c r="U75" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V75" s="16"/>
       <c r="W75" s="15"/>
       <c r="X75" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y75" s="16"/>
       <c r="Z75" s="15"/>
       <c r="AA75" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB75" s="16"/>
       <c r="AC75" s="15"/>
       <c r="AD75" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE75" s="16"/>
       <c r="AF75" s="15"/>
       <c r="AG75" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH75" s="16"/>
       <c r="AI75" s="15"/>
       <c r="AJ75" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK75" s="16"/>
       <c r="AL75" s="15"/>
       <c r="AM75" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN75" s="16"/>
       <c r="AO75" s="15"/>
       <c r="AP75" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ75" s="16"/>
       <c r="AR75" s="15"/>
       <c r="AS75" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT75" s="16"/>
       <c r="AU75" s="15"/>
       <c r="AV75" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW75" s="16"/>
       <c r="AX75" s="15"/>
       <c r="AY75" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ75" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ75" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA75" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA75" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7464,99 +7471,99 @@
       </c>
       <c r="H77" s="15"/>
       <c r="I77" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J77" s="16"/>
       <c r="K77" s="15"/>
       <c r="L77" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M77" s="16"/>
       <c r="N77" s="15"/>
       <c r="O77" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P77" s="16"/>
       <c r="Q77" s="15"/>
       <c r="R77" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S77" s="16"/>
       <c r="T77" s="15"/>
       <c r="U77" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V77" s="16"/>
       <c r="W77" s="15"/>
       <c r="X77" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y77" s="16"/>
       <c r="Z77" s="15"/>
       <c r="AA77" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB77" s="16"/>
       <c r="AC77" s="15"/>
       <c r="AD77" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE77" s="16"/>
       <c r="AF77" s="15"/>
       <c r="AG77" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH77" s="16"/>
       <c r="AI77" s="15"/>
       <c r="AJ77" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK77" s="16"/>
       <c r="AL77" s="15"/>
       <c r="AM77" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN77" s="16"/>
       <c r="AO77" s="15"/>
       <c r="AP77" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ77" s="16"/>
       <c r="AR77" s="15"/>
       <c r="AS77" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT77" s="16"/>
       <c r="AU77" s="15"/>
       <c r="AV77" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW77" s="16"/>
       <c r="AX77" s="15"/>
       <c r="AY77" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ77" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ77" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA77" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA77" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7635,99 +7642,99 @@
       </c>
       <c r="H79" s="15"/>
       <c r="I79" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J79" s="16"/>
       <c r="K79" s="15"/>
       <c r="L79" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M79" s="16"/>
       <c r="N79" s="15"/>
       <c r="O79" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P79" s="16"/>
       <c r="Q79" s="15"/>
       <c r="R79" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S79" s="16"/>
       <c r="T79" s="15"/>
       <c r="U79" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V79" s="16"/>
       <c r="W79" s="15"/>
       <c r="X79" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y79" s="16"/>
       <c r="Z79" s="15"/>
       <c r="AA79" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB79" s="16"/>
       <c r="AC79" s="15"/>
       <c r="AD79" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE79" s="16"/>
       <c r="AF79" s="15"/>
       <c r="AG79" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH79" s="16"/>
       <c r="AI79" s="15"/>
       <c r="AJ79" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK79" s="16"/>
       <c r="AL79" s="15"/>
       <c r="AM79" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN79" s="16"/>
       <c r="AO79" s="15"/>
       <c r="AP79" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ79" s="16"/>
       <c r="AR79" s="15"/>
       <c r="AS79" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT79" s="16"/>
       <c r="AU79" s="15"/>
       <c r="AV79" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW79" s="16"/>
       <c r="AX79" s="15"/>
       <c r="AY79" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ79" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ79" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA79" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA79" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7806,99 +7813,99 @@
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J81" s="16"/>
       <c r="K81" s="15"/>
       <c r="L81" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M81" s="16"/>
       <c r="N81" s="15"/>
       <c r="O81" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P81" s="16"/>
       <c r="Q81" s="15"/>
       <c r="R81" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S81" s="16"/>
       <c r="T81" s="15"/>
       <c r="U81" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V81" s="16"/>
       <c r="W81" s="15"/>
       <c r="X81" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y81" s="16"/>
       <c r="Z81" s="15"/>
       <c r="AA81" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB81" s="16"/>
       <c r="AC81" s="15"/>
       <c r="AD81" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE81" s="16"/>
       <c r="AF81" s="15"/>
       <c r="AG81" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH81" s="16"/>
       <c r="AI81" s="15"/>
       <c r="AJ81" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK81" s="16"/>
       <c r="AL81" s="15"/>
       <c r="AM81" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN81" s="16"/>
       <c r="AO81" s="15"/>
       <c r="AP81" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ81" s="16"/>
       <c r="AR81" s="15"/>
       <c r="AS81" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT81" s="16"/>
       <c r="AU81" s="15"/>
       <c r="AV81" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW81" s="16"/>
       <c r="AX81" s="15"/>
       <c r="AY81" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ81" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ81" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA81" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA81" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -7977,99 +7984,99 @@
       </c>
       <c r="H83" s="15"/>
       <c r="I83" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J83" s="16"/>
       <c r="K83" s="15"/>
       <c r="L83" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M83" s="16"/>
       <c r="N83" s="15"/>
       <c r="O83" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P83" s="16"/>
       <c r="Q83" s="15"/>
       <c r="R83" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S83" s="16"/>
       <c r="T83" s="15"/>
       <c r="U83" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V83" s="16"/>
       <c r="W83" s="15"/>
       <c r="X83" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y83" s="16"/>
       <c r="Z83" s="15"/>
       <c r="AA83" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB83" s="16"/>
       <c r="AC83" s="15"/>
       <c r="AD83" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE83" s="16"/>
       <c r="AF83" s="15"/>
       <c r="AG83" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH83" s="16"/>
       <c r="AI83" s="15"/>
       <c r="AJ83" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK83" s="16"/>
       <c r="AL83" s="15"/>
       <c r="AM83" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN83" s="16"/>
       <c r="AO83" s="15"/>
       <c r="AP83" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ83" s="16"/>
       <c r="AR83" s="15"/>
       <c r="AS83" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT83" s="16"/>
       <c r="AU83" s="15"/>
       <c r="AV83" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW83" s="16"/>
       <c r="AX83" s="15"/>
       <c r="AY83" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ83" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ83" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA83" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA83" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -8148,99 +8155,99 @@
       </c>
       <c r="H85" s="15"/>
       <c r="I85" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J85" s="16"/>
       <c r="K85" s="15"/>
       <c r="L85" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M85" s="16"/>
       <c r="N85" s="15"/>
       <c r="O85" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P85" s="16"/>
       <c r="Q85" s="15"/>
       <c r="R85" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S85" s="16"/>
       <c r="T85" s="15"/>
       <c r="U85" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V85" s="16"/>
       <c r="W85" s="15"/>
       <c r="X85" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y85" s="16"/>
       <c r="Z85" s="15"/>
       <c r="AA85" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB85" s="16"/>
       <c r="AC85" s="15"/>
       <c r="AD85" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE85" s="16"/>
       <c r="AF85" s="15"/>
       <c r="AG85" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH85" s="16"/>
       <c r="AI85" s="15"/>
       <c r="AJ85" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK85" s="16"/>
       <c r="AL85" s="15"/>
       <c r="AM85" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN85" s="16"/>
       <c r="AO85" s="15"/>
       <c r="AP85" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ85" s="16"/>
       <c r="AR85" s="15"/>
       <c r="AS85" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT85" s="16"/>
       <c r="AU85" s="15"/>
       <c r="AV85" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW85" s="16"/>
       <c r="AX85" s="15"/>
       <c r="AY85" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ85" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ85" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA85" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA85" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -8319,99 +8326,99 @@
       </c>
       <c r="H87" s="15"/>
       <c r="I87" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J87" s="16"/>
       <c r="K87" s="15"/>
       <c r="L87" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M87" s="16"/>
       <c r="N87" s="15"/>
       <c r="O87" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P87" s="16"/>
       <c r="Q87" s="15"/>
       <c r="R87" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S87" s="16"/>
       <c r="T87" s="15"/>
       <c r="U87" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V87" s="16"/>
       <c r="W87" s="15"/>
       <c r="X87" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y87" s="16"/>
       <c r="Z87" s="15"/>
       <c r="AA87" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB87" s="16"/>
       <c r="AC87" s="15"/>
       <c r="AD87" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE87" s="16"/>
       <c r="AF87" s="15"/>
       <c r="AG87" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH87" s="16"/>
       <c r="AI87" s="15"/>
       <c r="AJ87" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK87" s="16"/>
       <c r="AL87" s="15"/>
       <c r="AM87" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN87" s="16"/>
       <c r="AO87" s="15"/>
       <c r="AP87" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ87" s="16"/>
       <c r="AR87" s="15"/>
       <c r="AS87" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT87" s="16"/>
       <c r="AU87" s="15"/>
       <c r="AV87" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW87" s="16"/>
       <c r="AX87" s="15"/>
       <c r="AY87" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ87" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ87" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA87" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA87" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -8490,99 +8497,99 @@
       </c>
       <c r="H89" s="15"/>
       <c r="I89" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2</v>
       </c>
       <c r="J89" s="16"/>
       <c r="K89" s="15"/>
       <c r="L89" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2</v>
       </c>
       <c r="M89" s="16"/>
       <c r="N89" s="15"/>
       <c r="O89" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2</v>
       </c>
       <c r="P89" s="16"/>
       <c r="Q89" s="15"/>
       <c r="R89" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2</v>
       </c>
       <c r="S89" s="16"/>
       <c r="T89" s="15"/>
       <c r="U89" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2</v>
       </c>
       <c r="V89" s="16"/>
       <c r="W89" s="15"/>
       <c r="X89" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2</v>
       </c>
       <c r="Y89" s="16"/>
       <c r="Z89" s="15"/>
       <c r="AA89" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2</v>
       </c>
       <c r="AB89" s="16"/>
       <c r="AC89" s="15"/>
       <c r="AD89" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2</v>
       </c>
       <c r="AE89" s="16"/>
       <c r="AF89" s="15"/>
       <c r="AG89" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2</v>
       </c>
       <c r="AH89" s="16"/>
       <c r="AI89" s="15"/>
       <c r="AJ89" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2</v>
       </c>
       <c r="AK89" s="16"/>
       <c r="AL89" s="15"/>
       <c r="AM89" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2</v>
       </c>
       <c r="AN89" s="16"/>
       <c r="AO89" s="15"/>
       <c r="AP89" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2</v>
       </c>
       <c r="AQ89" s="16"/>
       <c r="AR89" s="15"/>
       <c r="AS89" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2</v>
       </c>
       <c r="AT89" s="16"/>
       <c r="AU89" s="15"/>
       <c r="AV89" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2</v>
       </c>
       <c r="AW89" s="16"/>
       <c r="AX89" s="15"/>
       <c r="AY89" s="15">
+        <f t="shared" si="338"/>
+        <v>2</v>
+      </c>
+      <c r="AZ89" s="17">
         <f t="shared" si="339"/>
-        <v>2</v>
-      </c>
-      <c r="AZ89" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA89" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA89" s="17">
-        <f t="shared" si="341"/>
         <v>2</v>
       </c>
     </row>
@@ -8659,99 +8666,99 @@
       </c>
       <c r="H91" s="15"/>
       <c r="I91" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>2.5</v>
       </c>
       <c r="J91" s="16"/>
       <c r="K91" s="15"/>
       <c r="L91" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>2.5</v>
       </c>
       <c r="M91" s="16"/>
       <c r="N91" s="15"/>
       <c r="O91" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>2.5</v>
       </c>
       <c r="P91" s="16"/>
       <c r="Q91" s="15"/>
       <c r="R91" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>2.5</v>
       </c>
       <c r="S91" s="16"/>
       <c r="T91" s="15"/>
       <c r="U91" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>2.5</v>
       </c>
       <c r="V91" s="16"/>
       <c r="W91" s="15"/>
       <c r="X91" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>2.5</v>
       </c>
       <c r="Y91" s="16"/>
       <c r="Z91" s="15"/>
       <c r="AA91" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>2.5</v>
       </c>
       <c r="AB91" s="16"/>
       <c r="AC91" s="15"/>
       <c r="AD91" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>2.5</v>
       </c>
       <c r="AE91" s="16"/>
       <c r="AF91" s="15"/>
       <c r="AG91" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>2.5</v>
       </c>
       <c r="AH91" s="16"/>
       <c r="AI91" s="15"/>
       <c r="AJ91" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>2.5</v>
       </c>
       <c r="AK91" s="16"/>
       <c r="AL91" s="15"/>
       <c r="AM91" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>2.5</v>
       </c>
       <c r="AN91" s="16"/>
       <c r="AO91" s="15"/>
       <c r="AP91" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>2.5</v>
       </c>
       <c r="AQ91" s="16"/>
       <c r="AR91" s="15"/>
       <c r="AS91" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>2.5</v>
       </c>
       <c r="AT91" s="16"/>
       <c r="AU91" s="15"/>
       <c r="AV91" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>2.5</v>
       </c>
       <c r="AW91" s="16"/>
       <c r="AX91" s="15"/>
       <c r="AY91" s="15">
+        <f t="shared" si="338"/>
+        <v>2.5</v>
+      </c>
+      <c r="AZ91" s="17">
         <f t="shared" si="339"/>
-        <v>2.5</v>
-      </c>
-      <c r="AZ91" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA91" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA91" s="17">
-        <f t="shared" si="341"/>
         <v>2.5</v>
       </c>
     </row>
@@ -8828,99 +8835,99 @@
       </c>
       <c r="H93" s="15"/>
       <c r="I93" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>1.5</v>
       </c>
       <c r="J93" s="16"/>
       <c r="K93" s="15"/>
       <c r="L93" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>1.5</v>
       </c>
       <c r="M93" s="16"/>
       <c r="N93" s="15"/>
       <c r="O93" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>1.5</v>
       </c>
       <c r="P93" s="16"/>
       <c r="Q93" s="15"/>
       <c r="R93" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>1.5</v>
       </c>
       <c r="S93" s="16"/>
       <c r="T93" s="15"/>
       <c r="U93" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>1.5</v>
       </c>
       <c r="V93" s="16"/>
       <c r="W93" s="15"/>
       <c r="X93" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>1.5</v>
       </c>
       <c r="Y93" s="16"/>
       <c r="Z93" s="15"/>
       <c r="AA93" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>1.5</v>
       </c>
       <c r="AB93" s="16"/>
       <c r="AC93" s="15"/>
       <c r="AD93" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>1.5</v>
       </c>
       <c r="AE93" s="16"/>
       <c r="AF93" s="15"/>
       <c r="AG93" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>1.5</v>
       </c>
       <c r="AH93" s="16"/>
       <c r="AI93" s="15"/>
       <c r="AJ93" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>1.5</v>
       </c>
       <c r="AK93" s="16"/>
       <c r="AL93" s="15"/>
       <c r="AM93" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>1.5</v>
       </c>
       <c r="AN93" s="16"/>
       <c r="AO93" s="15"/>
       <c r="AP93" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>1.5</v>
       </c>
       <c r="AQ93" s="16"/>
       <c r="AR93" s="15"/>
       <c r="AS93" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>1.5</v>
       </c>
       <c r="AT93" s="16"/>
       <c r="AU93" s="15"/>
       <c r="AV93" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>1.5</v>
       </c>
       <c r="AW93" s="16"/>
       <c r="AX93" s="15"/>
       <c r="AY93" s="15">
+        <f t="shared" si="338"/>
+        <v>1.5</v>
+      </c>
+      <c r="AZ93" s="17">
         <f t="shared" si="339"/>
-        <v>1.5</v>
-      </c>
-      <c r="AZ93" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA93" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA93" s="17">
-        <f t="shared" si="341"/>
         <v>1.5</v>
       </c>
     </row>
@@ -8987,99 +8994,99 @@
       <c r="G95" s="32"/>
       <c r="H95" s="15"/>
       <c r="I95" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>0</v>
       </c>
       <c r="J95" s="16"/>
       <c r="K95" s="15"/>
       <c r="L95" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>0</v>
       </c>
       <c r="M95" s="16"/>
       <c r="N95" s="15"/>
       <c r="O95" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>0</v>
       </c>
       <c r="P95" s="16"/>
       <c r="Q95" s="15"/>
       <c r="R95" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>0</v>
       </c>
       <c r="S95" s="16"/>
       <c r="T95" s="15"/>
       <c r="U95" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>0</v>
       </c>
       <c r="V95" s="16"/>
       <c r="W95" s="15"/>
       <c r="X95" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>0</v>
       </c>
       <c r="Y95" s="16"/>
       <c r="Z95" s="15"/>
       <c r="AA95" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>0</v>
       </c>
       <c r="AB95" s="16"/>
       <c r="AC95" s="15"/>
       <c r="AD95" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>0</v>
       </c>
       <c r="AE95" s="16"/>
       <c r="AF95" s="15"/>
       <c r="AG95" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>0</v>
       </c>
       <c r="AH95" s="16"/>
       <c r="AI95" s="15"/>
       <c r="AJ95" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>0</v>
       </c>
       <c r="AK95" s="16"/>
       <c r="AL95" s="15"/>
       <c r="AM95" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>0</v>
       </c>
       <c r="AN95" s="16"/>
       <c r="AO95" s="15"/>
       <c r="AP95" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>0</v>
       </c>
       <c r="AQ95" s="16"/>
       <c r="AR95" s="15"/>
       <c r="AS95" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>0</v>
       </c>
       <c r="AT95" s="16"/>
       <c r="AU95" s="15"/>
       <c r="AV95" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>0</v>
       </c>
       <c r="AW95" s="16"/>
       <c r="AX95" s="15"/>
       <c r="AY95" s="15">
+        <f t="shared" si="338"/>
+        <v>0</v>
+      </c>
+      <c r="AZ95" s="17">
         <f t="shared" si="339"/>
         <v>0</v>
       </c>
-      <c r="AZ95" s="17">
+      <c r="BA95" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA95" s="17">
-        <f t="shared" si="341"/>
         <v>0</v>
       </c>
     </row>
@@ -9146,99 +9153,99 @@
       <c r="G97" s="32"/>
       <c r="H97" s="15"/>
       <c r="I97" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>0</v>
       </c>
       <c r="J97" s="16"/>
       <c r="K97" s="15"/>
       <c r="L97" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>0</v>
       </c>
       <c r="M97" s="16"/>
       <c r="N97" s="15"/>
       <c r="O97" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>0</v>
       </c>
       <c r="P97" s="16"/>
       <c r="Q97" s="15"/>
       <c r="R97" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>0</v>
       </c>
       <c r="S97" s="16"/>
       <c r="T97" s="15"/>
       <c r="U97" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>0</v>
       </c>
       <c r="V97" s="16"/>
       <c r="W97" s="15"/>
       <c r="X97" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>0</v>
       </c>
       <c r="Y97" s="16"/>
       <c r="Z97" s="15"/>
       <c r="AA97" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>0</v>
       </c>
       <c r="AB97" s="16"/>
       <c r="AC97" s="15"/>
       <c r="AD97" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>0</v>
       </c>
       <c r="AE97" s="16"/>
       <c r="AF97" s="15"/>
       <c r="AG97" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>0</v>
       </c>
       <c r="AH97" s="16"/>
       <c r="AI97" s="15"/>
       <c r="AJ97" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>0</v>
       </c>
       <c r="AK97" s="16"/>
       <c r="AL97" s="15"/>
       <c r="AM97" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>0</v>
       </c>
       <c r="AN97" s="16"/>
       <c r="AO97" s="15"/>
       <c r="AP97" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>0</v>
       </c>
       <c r="AQ97" s="16"/>
       <c r="AR97" s="15"/>
       <c r="AS97" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>0</v>
       </c>
       <c r="AT97" s="16"/>
       <c r="AU97" s="15"/>
       <c r="AV97" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>0</v>
       </c>
       <c r="AW97" s="16"/>
       <c r="AX97" s="15"/>
       <c r="AY97" s="15">
+        <f t="shared" si="338"/>
+        <v>0</v>
+      </c>
+      <c r="AZ97" s="17">
         <f t="shared" si="339"/>
         <v>0</v>
       </c>
-      <c r="AZ97" s="17">
+      <c r="BA97" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA97" s="17">
-        <f t="shared" si="341"/>
         <v>0</v>
       </c>
     </row>
@@ -9305,99 +9312,99 @@
       <c r="G99" s="32"/>
       <c r="H99" s="15"/>
       <c r="I99" s="15">
-        <f t="shared" si="329"/>
+        <f t="shared" si="328"/>
         <v>0</v>
       </c>
       <c r="J99" s="16"/>
       <c r="K99" s="15"/>
       <c r="L99" s="15">
-        <f t="shared" si="342"/>
+        <f t="shared" si="341"/>
         <v>0</v>
       </c>
       <c r="M99" s="16"/>
       <c r="N99" s="15"/>
       <c r="O99" s="15">
-        <f t="shared" si="343"/>
+        <f t="shared" si="342"/>
         <v>0</v>
       </c>
       <c r="P99" s="16"/>
       <c r="Q99" s="15"/>
       <c r="R99" s="15">
-        <f t="shared" si="317"/>
+        <f t="shared" si="316"/>
         <v>0</v>
       </c>
       <c r="S99" s="16"/>
       <c r="T99" s="15"/>
       <c r="U99" s="15">
-        <f t="shared" si="318"/>
+        <f t="shared" si="317"/>
         <v>0</v>
       </c>
       <c r="V99" s="16"/>
       <c r="W99" s="15"/>
       <c r="X99" s="15">
-        <f t="shared" si="330"/>
+        <f t="shared" si="329"/>
         <v>0</v>
       </c>
       <c r="Y99" s="16"/>
       <c r="Z99" s="15"/>
       <c r="AA99" s="15">
-        <f t="shared" si="331"/>
+        <f t="shared" si="330"/>
         <v>0</v>
       </c>
       <c r="AB99" s="16"/>
       <c r="AC99" s="15"/>
       <c r="AD99" s="15">
-        <f t="shared" si="332"/>
+        <f t="shared" si="331"/>
         <v>0</v>
       </c>
       <c r="AE99" s="16"/>
       <c r="AF99" s="15"/>
       <c r="AG99" s="15">
-        <f t="shared" si="333"/>
+        <f t="shared" si="332"/>
         <v>0</v>
       </c>
       <c r="AH99" s="16"/>
       <c r="AI99" s="15"/>
       <c r="AJ99" s="15">
-        <f t="shared" si="334"/>
+        <f t="shared" si="333"/>
         <v>0</v>
       </c>
       <c r="AK99" s="16"/>
       <c r="AL99" s="15"/>
       <c r="AM99" s="15">
-        <f t="shared" si="335"/>
+        <f t="shared" si="334"/>
         <v>0</v>
       </c>
       <c r="AN99" s="16"/>
       <c r="AO99" s="15"/>
       <c r="AP99" s="15">
-        <f t="shared" si="336"/>
+        <f t="shared" si="335"/>
         <v>0</v>
       </c>
       <c r="AQ99" s="16"/>
       <c r="AR99" s="15"/>
       <c r="AS99" s="15">
-        <f t="shared" si="337"/>
+        <f t="shared" si="336"/>
         <v>0</v>
       </c>
       <c r="AT99" s="16"/>
       <c r="AU99" s="15"/>
       <c r="AV99" s="15">
-        <f t="shared" si="338"/>
+        <f t="shared" si="337"/>
         <v>0</v>
       </c>
       <c r="AW99" s="16"/>
       <c r="AX99" s="15"/>
       <c r="AY99" s="15">
+        <f t="shared" si="338"/>
+        <v>0</v>
+      </c>
+      <c r="AZ99" s="17">
         <f t="shared" si="339"/>
         <v>0</v>
       </c>
-      <c r="AZ99" s="17">
+      <c r="BA99" s="17">
         <f t="shared" si="340"/>
-        <v>0</v>
-      </c>
-      <c r="BA99" s="17">
-        <f t="shared" si="341"/>
         <v>0</v>
       </c>
     </row>
@@ -9456,6 +9463,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9467,11 +9479,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas de secuencia, actualización plantillas
Se añadieron los diagramas de secuencia del rubro de grupos, y se actualizó la plantilla de tareas y la de casos de uso en base a la elaboración de los diagramas de secuencia.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
+++ b/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668AE671-2173-4B99-A892-EA2283927C0F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8438D-C3C5-4E2D-B059-59FB908BF7D3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="106">
   <si>
     <t>Columna</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>En proceso</t>
-  </si>
-  <si>
-    <t>En Proceso</t>
   </si>
   <si>
     <t>CU-05</t>
@@ -1021,7 +1018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1032,13 +1029,13 @@
   <dimension ref="B1:BA100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AR58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AO6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="AS57" sqref="AS57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -2719,7 +2716,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="22" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>48</v>
       </c>
@@ -3417,7 +3414,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>54</v>
       </c>
@@ -3592,7 +3589,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="32" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>55</v>
       </c>
@@ -4451,7 +4448,7 @@
         <v>-0.19999999999999996</v>
       </c>
     </row>
-    <row r="42" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B42" s="29" t="s">
         <v>83</v>
       </c>
@@ -4626,7 +4623,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B44" s="29" t="s">
         <v>84</v>
       </c>
@@ -4801,7 +4798,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="46" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B46" s="29" t="s">
         <v>85</v>
       </c>
@@ -4978,10 +4975,10 @@
     </row>
     <row r="48" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B48" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="21"/>
@@ -5151,7 +5148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B50" s="29" t="s">
         <v>42</v>
       </c>
@@ -5219,7 +5216,7 @@
         <v>51</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G51" s="29">
         <v>2.5</v>
@@ -5298,30 +5295,32 @@
         <v>2.1</v>
       </c>
       <c r="AQ51" s="16"/>
-      <c r="AR51" s="15"/>
+      <c r="AR51" s="15">
+        <v>0.4</v>
+      </c>
       <c r="AS51" s="15">
         <f t="shared" ref="AS51" si="267">AP51-AR51</f>
-        <v>2.1</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="AT51" s="16"/>
       <c r="AU51" s="15"/>
       <c r="AV51" s="15">
         <f t="shared" ref="AV51" si="268">AS51-AU51</f>
-        <v>2.1</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="AW51" s="16"/>
       <c r="AX51" s="15"/>
       <c r="AY51" s="15">
         <f t="shared" ref="AY51" si="269">AV51-AX51</f>
-        <v>2.1</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="AZ51" s="17">
         <f>H51+K51+N51+Q51+T51+W51+Z51+AC51+AF51+AI51+AL51+AO51+AR51+AU51+AX51</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="BA51" s="17">
         <f>G51-AZ51</f>
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="52" spans="2:53" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -5392,7 +5391,7 @@
         <v>51</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="G53" s="29">
         <v>2.5</v>
@@ -5471,27 +5470,29 @@
         <v>2</v>
       </c>
       <c r="AQ53" s="16"/>
-      <c r="AR53" s="15"/>
+      <c r="AR53" s="15">
+        <v>0.25</v>
+      </c>
       <c r="AS53" s="15">
         <f t="shared" ref="AS53" si="279">AP53-AR53</f>
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="AT53" s="16"/>
       <c r="AU53" s="15"/>
       <c r="AV53" s="15">
         <f t="shared" ref="AV53" si="280">AS53-AU53</f>
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="AW53" s="16"/>
       <c r="AX53" s="15"/>
       <c r="AY53" s="15"/>
       <c r="AZ53" s="17">
         <f>H53+K53+N53+Q53+T53+W53+Z53+AC53+AF53+AI53+AL53+AO53+AR53+AU53+AX53</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="BA53" s="17">
         <f>G53-AZ53</f>
-        <v>2</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="54" spans="2:53" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5562,7 +5563,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G55" s="29">
         <v>2.5</v>
@@ -5641,30 +5642,32 @@
         <v>2.1</v>
       </c>
       <c r="AQ55" s="16"/>
-      <c r="AR55" s="15"/>
+      <c r="AR55" s="15">
+        <v>0.5</v>
+      </c>
       <c r="AS55" s="15">
         <f t="shared" ref="AS55" si="290">AP55-AR55</f>
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
       <c r="AT55" s="16"/>
       <c r="AU55" s="15"/>
       <c r="AV55" s="15">
         <f t="shared" ref="AV55" si="291">AS55-AU55</f>
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
       <c r="AW55" s="16"/>
       <c r="AX55" s="15"/>
       <c r="AY55" s="15">
         <f t="shared" ref="AY55" si="292">AV55-AX55</f>
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
       <c r="AZ55" s="17">
         <f>H55+K55+N55+Q55+T55+W55+Z55+AC55+AF55+AI55+AL55+AO55+AR55+AU55+AX55</f>
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="BA55" s="17">
         <f>G55-AZ55</f>
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="56" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
@@ -5735,7 +5738,7 @@
         <v>51</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="G57" s="29">
         <v>2.5</v>
@@ -5816,33 +5819,35 @@
         <v>1</v>
       </c>
       <c r="AQ57" s="16"/>
-      <c r="AR57" s="15"/>
+      <c r="AR57" s="15">
+        <v>0.48</v>
+      </c>
       <c r="AS57" s="15">
         <f t="shared" ref="AS57" si="302">AP57-AR57</f>
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="AT57" s="16"/>
       <c r="AU57" s="15"/>
       <c r="AV57" s="15">
         <f t="shared" ref="AV57" si="303">AS57-AU57</f>
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="AW57" s="16"/>
       <c r="AX57" s="15"/>
       <c r="AY57" s="15">
         <f t="shared" ref="AY57" si="304">AV57-AX57</f>
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="AZ57" s="17">
         <f>H57+K57+N57+Q57+T57+W57+Z57+AC57+AF57+AI57+AL57+AO57+AR57+AU57+AX57</f>
-        <v>1.5</v>
+        <v>1.98</v>
       </c>
       <c r="BA57" s="17">
         <f>G57-AZ57</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:53" x14ac:dyDescent="0.25">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B58" s="29" t="s">
         <v>86</v>
       </c>
@@ -6712,7 +6717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B68" s="29" t="s">
         <v>84</v>
       </c>
@@ -6883,7 +6888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
         <v>85</v>
       </c>
@@ -7054,7 +7059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B72" s="29" t="s">
         <v>41</v>
       </c>
@@ -7225,7 +7230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:53" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B74" s="29" t="s">
         <v>42</v>
       </c>
@@ -7567,7 +7572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B78" s="29" t="s">
         <v>44</v>
       </c>
@@ -8251,7 +8256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B86" s="29" t="s">
         <v>88</v>
       </c>
@@ -8593,7 +8598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B90" s="20"/>
       <c r="C90" s="18" t="s">
         <v>99</v>
@@ -9463,11 +9468,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9479,6 +9479,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -9503,7 +9508,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Creación de ventanas en netbeans y registros de tiempos
En este commit se crearon las ventanas en netbeans para su posterior codificación y se registraron los tiempos que tomaron en elobrarlas
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
+++ b/Plantillas/Entrega 2/Plantilla Lista de Tareas de la Entrega 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8438D-C3C5-4E2D-B059-59FB908BF7D3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089566B2-1C45-43DF-8BE4-B1A523B1F5E5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1018,7 +1018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1029,13 +1029,13 @@
   <dimension ref="B1:BA100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AO6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AK82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AS57" sqref="AS57"/>
+      <selection pane="bottomRight" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -7982,7 +7982,7 @@
         <v>76</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G83" s="32">
         <v>2</v>
@@ -8053,36 +8053,38 @@
         <v>2</v>
       </c>
       <c r="AN83" s="16"/>
-      <c r="AO83" s="15"/>
+      <c r="AO83" s="15">
+        <v>1.5</v>
+      </c>
       <c r="AP83" s="15">
         <f t="shared" si="335"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AQ83" s="16"/>
       <c r="AR83" s="15"/>
       <c r="AS83" s="15">
         <f t="shared" si="336"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AT83" s="16"/>
       <c r="AU83" s="15"/>
       <c r="AV83" s="15">
         <f t="shared" si="337"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AW83" s="16"/>
       <c r="AX83" s="15"/>
       <c r="AY83" s="15">
         <f t="shared" si="338"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AZ83" s="17">
         <f t="shared" si="339"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA83" s="17">
         <f t="shared" si="340"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84" spans="2:53" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -8153,7 +8155,7 @@
         <v>76</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G85" s="32">
         <v>2</v>
@@ -8324,7 +8326,7 @@
         <v>76</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G87" s="32">
         <v>2</v>
@@ -8401,30 +8403,32 @@
         <v>2</v>
       </c>
       <c r="AQ87" s="16"/>
-      <c r="AR87" s="15"/>
+      <c r="AR87" s="15">
+        <v>0.5</v>
+      </c>
       <c r="AS87" s="15">
         <f t="shared" si="336"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AT87" s="16"/>
       <c r="AU87" s="15"/>
       <c r="AV87" s="15">
         <f t="shared" si="337"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AW87" s="16"/>
       <c r="AX87" s="15"/>
       <c r="AY87" s="15">
         <f t="shared" si="338"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AZ87" s="17">
         <f t="shared" si="339"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA87" s="17">
         <f t="shared" si="340"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="88" spans="2:53" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8495,7 +8499,7 @@
         <v>76</v>
       </c>
       <c r="F89" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G89" s="32">
         <v>2</v>
@@ -8572,30 +8576,32 @@
         <v>2</v>
       </c>
       <c r="AQ89" s="16"/>
-      <c r="AR89" s="15"/>
+      <c r="AR89" s="15">
+        <v>0.5</v>
+      </c>
       <c r="AS89" s="15">
         <f t="shared" si="336"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AT89" s="16"/>
       <c r="AU89" s="15"/>
       <c r="AV89" s="15">
         <f t="shared" si="337"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AW89" s="16"/>
       <c r="AX89" s="15"/>
       <c r="AY89" s="15">
         <f t="shared" si="338"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AZ89" s="17">
         <f t="shared" si="339"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA89" s="17">
         <f t="shared" si="340"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="90" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
@@ -9468,6 +9474,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9479,11 +9490,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -9508,7 +9514,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>

</xml_diff>